<commit_message>
Updating Montville, just raw data, does not effect final processed data.
</commit_message>
<xml_diff>
--- a/raw/Grand List Data revised 5-2017.xlsx
+++ b/raw/Grand List Data revised 5-2017.xlsx
@@ -2615,7 +2615,7 @@
     <t xml:space="preserve">Montville Power LLC</t>
   </si>
   <si>
-    <t xml:space="preserve">Westbrook Converting Co</t>
+    <t xml:space="preserve">WestRock Converting Co</t>
   </si>
   <si>
     <t xml:space="preserve">Home Depot USA Inc.</t>
@@ -6531,17 +6531,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="169" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="170" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="169" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6590,19 +6589,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -6665,13 +6651,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6740,38 +6726,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6804,7 +6758,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6828,35 +6782,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6888,11 +6814,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6924,7 +6846,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6948,44 +6870,45 @@
   <dimension ref="A1:IW196"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E169" activeCellId="0" sqref="E169"/>
+      <selection pane="bottomLeft" activeCell="K87" activeCellId="0" sqref="K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.61224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8276,91 +8199,91 @@
         <v>42150</v>
       </c>
     </row>
-    <row r="16" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="n">
+    <row r="16" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D16" s="19" t="n">
+      <c r="D16" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="17" t="n">
+      <c r="F16" s="2" t="n">
         <v>287401220</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H16" s="17" t="n">
+      <c r="H16" s="2" t="n">
         <v>134169652</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J16" s="20" t="n">
+      <c r="J16" s="5" t="n">
         <v>109100930</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L16" s="17" t="n">
+      <c r="L16" s="2" t="n">
         <v>50683490</v>
       </c>
-      <c r="M16" s="17" t="s">
+      <c r="M16" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="N16" s="17" t="n">
+      <c r="N16" s="2" t="n">
         <v>47187434</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="O16" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="P16" s="17" t="n">
+      <c r="P16" s="2" t="n">
         <v>42240280</v>
       </c>
-      <c r="Q16" s="17" t="s">
+      <c r="Q16" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="R16" s="17" t="n">
+      <c r="R16" s="2" t="n">
         <v>37834440</v>
       </c>
-      <c r="S16" s="17" t="s">
+      <c r="S16" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="T16" s="17" t="n">
+      <c r="T16" s="2" t="n">
         <v>34728720</v>
       </c>
-      <c r="U16" s="17" t="s">
+      <c r="U16" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="V16" s="17" t="n">
+      <c r="V16" s="2" t="n">
         <v>25411070</v>
       </c>
-      <c r="W16" s="17" t="s">
+      <c r="W16" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="X16" s="17" t="n">
+      <c r="X16" s="2" t="n">
         <v>23884974</v>
       </c>
-      <c r="Y16" s="20" t="n">
+      <c r="Y16" s="5" t="n">
         <f aca="false">SUM(E16:X16)</f>
         <v>792642210</v>
       </c>
-      <c r="Z16" s="22" t="n">
+      <c r="Z16" s="6" t="n">
         <v>2016</v>
       </c>
-      <c r="AA16" s="17" t="n">
+      <c r="AA16" s="2" t="n">
         <v>8415459165</v>
       </c>
-      <c r="AB16" s="17" t="n">
+      <c r="AB16" s="2" t="n">
         <v>6024684505</v>
       </c>
-      <c r="AC16" s="23" t="n">
+      <c r="AC16" s="7" t="n">
         <v>42888</v>
       </c>
     </row>
@@ -10884,42 +10807,42 @@
         <v>42208</v>
       </c>
     </row>
-    <row r="46" s="30" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="25" t="n">
+    <row r="46" s="22" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="25" t="s">
+      <c r="B46" s="18"/>
+      <c r="C46" s="17" t="s">
         <v>467</v>
       </c>
       <c r="D46" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="E46" s="27" t="s">
+      <c r="E46" s="19" t="s">
         <v>468</v>
       </c>
       <c r="F46" s="5" t="n">
         <v>23790010</v>
       </c>
-      <c r="G46" s="27" t="s">
+      <c r="G46" s="19" t="s">
         <v>469</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>21834220</v>
       </c>
-      <c r="I46" s="27" t="s">
+      <c r="I46" s="19" t="s">
         <v>470</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>19261970</v>
       </c>
-      <c r="K46" s="27" t="s">
+      <c r="K46" s="19" t="s">
         <v>471</v>
       </c>
-      <c r="L46" s="28" t="n">
+      <c r="L46" s="20" t="n">
         <v>15501520</v>
       </c>
-      <c r="M46" s="27" t="s">
+      <c r="M46" s="19" t="s">
         <v>472</v>
       </c>
       <c r="N46" s="5" t="n">
@@ -10931,28 +10854,28 @@
       <c r="P46" s="5" t="n">
         <v>11063090</v>
       </c>
-      <c r="Q46" s="27" t="s">
+      <c r="Q46" s="19" t="s">
         <v>101</v>
       </c>
       <c r="R46" s="5" t="n">
         <v>10990100</v>
       </c>
-      <c r="S46" s="27" t="s">
+      <c r="S46" s="19" t="s">
         <v>473</v>
       </c>
       <c r="T46" s="5" t="n">
         <v>9135090</v>
       </c>
-      <c r="U46" s="27" t="s">
+      <c r="U46" s="19" t="s">
         <v>474</v>
       </c>
       <c r="V46" s="5" t="n">
         <v>8776440</v>
       </c>
-      <c r="W46" s="27" t="s">
+      <c r="W46" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="X46" s="28" t="n">
+      <c r="X46" s="20" t="n">
         <v>8184460</v>
       </c>
       <c r="Y46" s="5" t="n">
@@ -10968,7 +10891,7 @@
       <c r="AB46" s="5" t="n">
         <v>962146920</v>
       </c>
-      <c r="AC46" s="29" t="n">
+      <c r="AC46" s="21" t="n">
         <v>42880</v>
       </c>
     </row>
@@ -11573,7 +11496,7 @@
       <c r="AA53" s="5" t="n">
         <v>3664627838</v>
       </c>
-      <c r="AB53" s="31" t="n">
+      <c r="AB53" s="23" t="n">
         <v>3595959571</v>
       </c>
       <c r="AC53" s="7" t="n">
@@ -12085,7 +12008,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="24" t="s">
         <v>602</v>
       </c>
       <c r="D60" s="3" t="n">
@@ -12335,7 +12258,7 @@
       <c r="AA62" s="11" t="n">
         <v>904391025</v>
       </c>
-      <c r="AB62" s="33" t="n">
+      <c r="AB62" s="25" t="n">
         <v>901419307</v>
       </c>
       <c r="AC62" s="14" t="n">
@@ -12528,7 +12451,7 @@
       <c r="E65" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F65" s="34" t="n">
+      <c r="F65" s="26" t="n">
         <v>139442670</v>
       </c>
       <c r="G65" s="9" t="s">
@@ -12552,28 +12475,28 @@
       <c r="M65" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="N65" s="34" t="n">
+      <c r="N65" s="26" t="n">
         <v>48977640</v>
       </c>
-      <c r="O65" s="35" t="s">
+      <c r="O65" s="27" t="s">
         <v>658</v>
       </c>
       <c r="P65" s="11" t="n">
         <v>45400500</v>
       </c>
-      <c r="Q65" s="35" t="s">
+      <c r="Q65" s="27" t="s">
         <v>659</v>
       </c>
       <c r="R65" s="11" t="n">
         <v>44450000</v>
       </c>
-      <c r="S65" s="35" t="s">
+      <c r="S65" s="27" t="s">
         <v>660</v>
       </c>
       <c r="T65" s="11" t="n">
         <v>35652810</v>
       </c>
-      <c r="U65" s="35" t="s">
+      <c r="U65" s="27" t="s">
         <v>661</v>
       </c>
       <c r="V65" s="11" t="n">
@@ -12595,7 +12518,7 @@
       <c r="AA65" s="11" t="n">
         <v>3621429969</v>
       </c>
-      <c r="AB65" s="36" t="n">
+      <c r="AB65" s="28" t="n">
         <v>3535402755</v>
       </c>
       <c r="AC65" s="14" t="n">
@@ -12962,7 +12885,7 @@
       <c r="E70" s="9" t="s">
         <v>702</v>
       </c>
-      <c r="F70" s="37" t="n">
+      <c r="F70" s="29" t="n">
         <v>109936552</v>
       </c>
       <c r="G70" s="9" t="s">
@@ -13022,7 +12945,7 @@
       <c r="Z70" s="13" t="n">
         <v>2014</v>
       </c>
-      <c r="AA70" s="38" t="n">
+      <c r="AA70" s="30" t="n">
         <v>1527677336</v>
       </c>
       <c r="AB70" s="11" t="n">
@@ -13465,7 +13388,7 @@
       <c r="AA75" s="5" t="n">
         <v>1036999800</v>
       </c>
-      <c r="AB75" s="31" t="n">
+      <c r="AB75" s="23" t="n">
         <v>1033225640</v>
       </c>
       <c r="AC75" s="7" t="n">
@@ -13560,319 +13483,319 @@
         <v>42829</v>
       </c>
     </row>
-    <row r="77" s="43" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="39" t="n">
+    <row r="77" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B77" s="40"/>
-      <c r="C77" s="39" t="s">
+      <c r="B77" s="16"/>
+      <c r="C77" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="D77" s="41" t="n">
+      <c r="D77" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="E77" s="39" t="s">
+      <c r="E77" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F77" s="42" t="n">
+      <c r="F77" s="5" t="n">
         <v>28527310</v>
       </c>
-      <c r="G77" s="39" t="s">
+      <c r="G77" s="2" t="s">
         <v>765</v>
       </c>
-      <c r="H77" s="42" t="n">
+      <c r="H77" s="5" t="n">
         <v>8966200</v>
       </c>
-      <c r="I77" s="39" t="s">
+      <c r="I77" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="J77" s="42" t="n">
+      <c r="J77" s="5" t="n">
         <v>6295800</v>
       </c>
-      <c r="K77" s="39" t="s">
+      <c r="K77" s="2" t="s">
         <v>767</v>
       </c>
-      <c r="L77" s="42" t="n">
+      <c r="L77" s="5" t="n">
         <v>6260100</v>
       </c>
-      <c r="M77" s="39" t="s">
+      <c r="M77" s="2" t="s">
         <v>768</v>
       </c>
-      <c r="N77" s="42" t="n">
+      <c r="N77" s="5" t="n">
         <v>5862200</v>
       </c>
-      <c r="O77" s="39" t="s">
+      <c r="O77" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="P77" s="42" t="n">
+      <c r="P77" s="5" t="n">
         <v>5590680</v>
       </c>
-      <c r="Q77" s="39" t="s">
+      <c r="Q77" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="R77" s="42" t="n">
+      <c r="R77" s="5" t="n">
         <v>5460000</v>
       </c>
-      <c r="S77" s="39" t="s">
+      <c r="S77" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="T77" s="42" t="n">
+      <c r="T77" s="5" t="n">
         <v>5447790</v>
       </c>
-      <c r="U77" s="43" t="s">
+      <c r="U77" s="31" t="s">
         <v>771</v>
       </c>
-      <c r="V77" s="43" t="n">
+      <c r="V77" s="31" t="n">
         <v>5441080</v>
       </c>
-      <c r="W77" s="39" t="s">
+      <c r="W77" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="X77" s="42" t="n">
+      <c r="X77" s="5" t="n">
         <v>5262700</v>
       </c>
-      <c r="Y77" s="42" t="n">
+      <c r="Y77" s="5" t="n">
         <f aca="false">SUM(E77:X77)</f>
         <v>83113860</v>
       </c>
-      <c r="Z77" s="44" t="n">
+      <c r="Z77" s="6" t="n">
         <v>2016</v>
       </c>
-      <c r="AA77" s="42"/>
-      <c r="AB77" s="42"/>
-      <c r="AC77" s="45" t="n">
+      <c r="AA77" s="5"/>
+      <c r="AB77" s="5"/>
+      <c r="AC77" s="7" t="n">
         <v>42922</v>
       </c>
-      <c r="AD77" s="46"/>
-      <c r="AE77" s="46"/>
-      <c r="AF77" s="46" t="n">
+      <c r="AD77" s="8"/>
+      <c r="AE77" s="8"/>
+      <c r="AF77" s="8" t="n">
         <v>2452713700</v>
       </c>
-      <c r="AG77" s="46"/>
-      <c r="AH77" s="46"/>
-      <c r="AI77" s="46"/>
-      <c r="AJ77" s="46"/>
-      <c r="AK77" s="46"/>
-      <c r="AL77" s="46"/>
-      <c r="AM77" s="46"/>
-      <c r="AN77" s="46"/>
-      <c r="AO77" s="46"/>
-      <c r="AP77" s="46"/>
-      <c r="AQ77" s="46"/>
-      <c r="AR77" s="46"/>
-      <c r="AS77" s="46"/>
-      <c r="AT77" s="46"/>
-      <c r="AU77" s="46"/>
-      <c r="AV77" s="46"/>
-      <c r="AW77" s="46"/>
-      <c r="AX77" s="46"/>
-      <c r="AY77" s="46"/>
-      <c r="AZ77" s="46"/>
-      <c r="BA77" s="46"/>
-      <c r="BB77" s="46"/>
-      <c r="BC77" s="46"/>
-      <c r="BD77" s="46"/>
-      <c r="BE77" s="46"/>
-      <c r="BF77" s="46"/>
-      <c r="BG77" s="46"/>
-      <c r="BH77" s="46"/>
-      <c r="BI77" s="46"/>
-      <c r="BJ77" s="46"/>
-      <c r="BK77" s="46"/>
-      <c r="BL77" s="46"/>
-      <c r="BM77" s="46"/>
-      <c r="BN77" s="46"/>
-      <c r="BO77" s="46"/>
-      <c r="BP77" s="46"/>
-      <c r="BQ77" s="46"/>
-      <c r="BR77" s="46"/>
-      <c r="BS77" s="46"/>
-      <c r="BT77" s="46"/>
-      <c r="BU77" s="46"/>
-      <c r="BV77" s="46"/>
-      <c r="BW77" s="46"/>
-      <c r="BX77" s="46"/>
-      <c r="BY77" s="46"/>
-      <c r="BZ77" s="46"/>
-      <c r="CA77" s="46"/>
-      <c r="CB77" s="46"/>
-      <c r="CC77" s="46"/>
-      <c r="CD77" s="46"/>
-      <c r="CE77" s="46"/>
-      <c r="CF77" s="46"/>
-      <c r="CG77" s="46"/>
-      <c r="CH77" s="46"/>
-      <c r="CI77" s="46"/>
-      <c r="CJ77" s="46"/>
-      <c r="CK77" s="46"/>
-      <c r="CL77" s="46"/>
-      <c r="CM77" s="46"/>
-      <c r="CN77" s="46"/>
-      <c r="CO77" s="46"/>
-      <c r="CP77" s="46"/>
-      <c r="CQ77" s="46"/>
-      <c r="CR77" s="46"/>
-      <c r="CS77" s="46"/>
-      <c r="CT77" s="46"/>
-      <c r="CU77" s="46"/>
-      <c r="CV77" s="46"/>
-      <c r="CW77" s="46"/>
-      <c r="CX77" s="46"/>
-      <c r="CY77" s="46"/>
-      <c r="CZ77" s="46"/>
-      <c r="DA77" s="46"/>
-      <c r="DB77" s="46"/>
-      <c r="DC77" s="46"/>
-      <c r="DD77" s="46"/>
-      <c r="DE77" s="46"/>
-      <c r="DF77" s="46"/>
-      <c r="DG77" s="46"/>
-      <c r="DH77" s="46"/>
-      <c r="DI77" s="46"/>
-      <c r="DJ77" s="46"/>
-      <c r="DK77" s="46"/>
-      <c r="DL77" s="46"/>
-      <c r="DM77" s="46"/>
-      <c r="DN77" s="46"/>
-      <c r="DO77" s="46"/>
-      <c r="DP77" s="46"/>
-      <c r="DQ77" s="46"/>
-      <c r="DR77" s="46"/>
-      <c r="DS77" s="46"/>
-      <c r="DT77" s="46"/>
-      <c r="DU77" s="46"/>
-      <c r="DV77" s="46"/>
-      <c r="DW77" s="46"/>
-      <c r="DX77" s="46"/>
-      <c r="DY77" s="46"/>
-      <c r="DZ77" s="46"/>
-      <c r="EA77" s="46"/>
-      <c r="EB77" s="46"/>
-      <c r="EC77" s="46"/>
-      <c r="ED77" s="46"/>
-      <c r="EE77" s="46"/>
-      <c r="EF77" s="46"/>
-      <c r="EG77" s="46"/>
-      <c r="EH77" s="46"/>
-      <c r="EI77" s="46"/>
-      <c r="EJ77" s="46"/>
-      <c r="EK77" s="46"/>
-      <c r="EL77" s="46"/>
-      <c r="EM77" s="46"/>
-      <c r="EN77" s="46"/>
-      <c r="EO77" s="46"/>
-      <c r="EP77" s="46"/>
-      <c r="EQ77" s="46"/>
-      <c r="ER77" s="46"/>
-      <c r="ES77" s="46"/>
-      <c r="ET77" s="46"/>
-      <c r="EU77" s="46"/>
-      <c r="EV77" s="46"/>
-      <c r="EW77" s="46"/>
-      <c r="EX77" s="46"/>
-      <c r="EY77" s="46"/>
-      <c r="EZ77" s="46"/>
-      <c r="FA77" s="46"/>
-      <c r="FB77" s="46"/>
-      <c r="FC77" s="46"/>
-      <c r="FD77" s="46"/>
-      <c r="FE77" s="46"/>
-      <c r="FF77" s="46"/>
-      <c r="FG77" s="46"/>
-      <c r="FH77" s="46"/>
-      <c r="FI77" s="46"/>
-      <c r="FJ77" s="46"/>
-      <c r="FK77" s="46"/>
-      <c r="FL77" s="46"/>
-      <c r="FM77" s="46"/>
-      <c r="FN77" s="46"/>
-      <c r="FO77" s="46"/>
-      <c r="FP77" s="46"/>
-      <c r="FQ77" s="46"/>
-      <c r="FR77" s="46"/>
-      <c r="FS77" s="46"/>
-      <c r="FT77" s="46"/>
-      <c r="FU77" s="46"/>
-      <c r="FV77" s="46"/>
-      <c r="FW77" s="46"/>
-      <c r="FX77" s="46"/>
-      <c r="FY77" s="46"/>
-      <c r="FZ77" s="46"/>
-      <c r="GA77" s="46"/>
-      <c r="GB77" s="46"/>
-      <c r="GC77" s="46"/>
-      <c r="GD77" s="46"/>
-      <c r="GE77" s="46"/>
-      <c r="GF77" s="46"/>
-      <c r="GG77" s="46"/>
-      <c r="GH77" s="46"/>
-      <c r="GI77" s="46"/>
-      <c r="GJ77" s="46"/>
-      <c r="GK77" s="46"/>
-      <c r="GL77" s="46"/>
-      <c r="GM77" s="46"/>
-      <c r="GN77" s="46"/>
-      <c r="GO77" s="46"/>
-      <c r="GP77" s="46"/>
-      <c r="GQ77" s="46"/>
-      <c r="GR77" s="46"/>
-      <c r="GS77" s="46"/>
-      <c r="GT77" s="46"/>
-      <c r="GU77" s="46"/>
-      <c r="GV77" s="46"/>
-      <c r="GW77" s="46"/>
-      <c r="GX77" s="46"/>
-      <c r="GY77" s="46"/>
-      <c r="GZ77" s="46"/>
-      <c r="HA77" s="46"/>
-      <c r="HB77" s="46"/>
-      <c r="HC77" s="46"/>
-      <c r="HD77" s="46"/>
-      <c r="HE77" s="46"/>
-      <c r="HF77" s="46"/>
-      <c r="HG77" s="46"/>
-      <c r="HH77" s="46"/>
-      <c r="HI77" s="46"/>
-      <c r="HJ77" s="46"/>
-      <c r="HK77" s="46"/>
-      <c r="HL77" s="46"/>
-      <c r="HM77" s="46"/>
-      <c r="HN77" s="46"/>
-      <c r="HO77" s="46"/>
-      <c r="HP77" s="46"/>
-      <c r="HQ77" s="46"/>
-      <c r="HR77" s="46"/>
-      <c r="HS77" s="46"/>
-      <c r="HT77" s="46"/>
-      <c r="HU77" s="46"/>
-      <c r="HV77" s="46"/>
-      <c r="HW77" s="46"/>
-      <c r="HX77" s="46"/>
-      <c r="HY77" s="46"/>
-      <c r="HZ77" s="46"/>
-      <c r="IA77" s="46"/>
-      <c r="IB77" s="46"/>
-      <c r="IC77" s="46"/>
-      <c r="ID77" s="46"/>
-      <c r="IE77" s="46"/>
-      <c r="IF77" s="46"/>
-      <c r="IG77" s="46"/>
-      <c r="IH77" s="46"/>
-      <c r="II77" s="46"/>
-      <c r="IJ77" s="46"/>
-      <c r="IK77" s="46"/>
-      <c r="IL77" s="46"/>
-      <c r="IM77" s="46"/>
-      <c r="IN77" s="46"/>
-      <c r="IO77" s="46"/>
-      <c r="IP77" s="46"/>
-      <c r="IQ77" s="46"/>
-      <c r="IR77" s="46"/>
-      <c r="IS77" s="46"/>
-      <c r="IT77" s="46"/>
-      <c r="IU77" s="46"/>
-      <c r="IV77" s="46"/>
-      <c r="IW77" s="46"/>
+      <c r="AG77" s="8"/>
+      <c r="AH77" s="8"/>
+      <c r="AI77" s="8"/>
+      <c r="AJ77" s="8"/>
+      <c r="AK77" s="8"/>
+      <c r="AL77" s="8"/>
+      <c r="AM77" s="8"/>
+      <c r="AN77" s="8"/>
+      <c r="AO77" s="8"/>
+      <c r="AP77" s="8"/>
+      <c r="AQ77" s="8"/>
+      <c r="AR77" s="8"/>
+      <c r="AS77" s="8"/>
+      <c r="AT77" s="8"/>
+      <c r="AU77" s="8"/>
+      <c r="AV77" s="8"/>
+      <c r="AW77" s="8"/>
+      <c r="AX77" s="8"/>
+      <c r="AY77" s="8"/>
+      <c r="AZ77" s="8"/>
+      <c r="BA77" s="8"/>
+      <c r="BB77" s="8"/>
+      <c r="BC77" s="8"/>
+      <c r="BD77" s="8"/>
+      <c r="BE77" s="8"/>
+      <c r="BF77" s="8"/>
+      <c r="BG77" s="8"/>
+      <c r="BH77" s="8"/>
+      <c r="BI77" s="8"/>
+      <c r="BJ77" s="8"/>
+      <c r="BK77" s="8"/>
+      <c r="BL77" s="8"/>
+      <c r="BM77" s="8"/>
+      <c r="BN77" s="8"/>
+      <c r="BO77" s="8"/>
+      <c r="BP77" s="8"/>
+      <c r="BQ77" s="8"/>
+      <c r="BR77" s="8"/>
+      <c r="BS77" s="8"/>
+      <c r="BT77" s="8"/>
+      <c r="BU77" s="8"/>
+      <c r="BV77" s="8"/>
+      <c r="BW77" s="8"/>
+      <c r="BX77" s="8"/>
+      <c r="BY77" s="8"/>
+      <c r="BZ77" s="8"/>
+      <c r="CA77" s="8"/>
+      <c r="CB77" s="8"/>
+      <c r="CC77" s="8"/>
+      <c r="CD77" s="8"/>
+      <c r="CE77" s="8"/>
+      <c r="CF77" s="8"/>
+      <c r="CG77" s="8"/>
+      <c r="CH77" s="8"/>
+      <c r="CI77" s="8"/>
+      <c r="CJ77" s="8"/>
+      <c r="CK77" s="8"/>
+      <c r="CL77" s="8"/>
+      <c r="CM77" s="8"/>
+      <c r="CN77" s="8"/>
+      <c r="CO77" s="8"/>
+      <c r="CP77" s="8"/>
+      <c r="CQ77" s="8"/>
+      <c r="CR77" s="8"/>
+      <c r="CS77" s="8"/>
+      <c r="CT77" s="8"/>
+      <c r="CU77" s="8"/>
+      <c r="CV77" s="8"/>
+      <c r="CW77" s="8"/>
+      <c r="CX77" s="8"/>
+      <c r="CY77" s="8"/>
+      <c r="CZ77" s="8"/>
+      <c r="DA77" s="8"/>
+      <c r="DB77" s="8"/>
+      <c r="DC77" s="8"/>
+      <c r="DD77" s="8"/>
+      <c r="DE77" s="8"/>
+      <c r="DF77" s="8"/>
+      <c r="DG77" s="8"/>
+      <c r="DH77" s="8"/>
+      <c r="DI77" s="8"/>
+      <c r="DJ77" s="8"/>
+      <c r="DK77" s="8"/>
+      <c r="DL77" s="8"/>
+      <c r="DM77" s="8"/>
+      <c r="DN77" s="8"/>
+      <c r="DO77" s="8"/>
+      <c r="DP77" s="8"/>
+      <c r="DQ77" s="8"/>
+      <c r="DR77" s="8"/>
+      <c r="DS77" s="8"/>
+      <c r="DT77" s="8"/>
+      <c r="DU77" s="8"/>
+      <c r="DV77" s="8"/>
+      <c r="DW77" s="8"/>
+      <c r="DX77" s="8"/>
+      <c r="DY77" s="8"/>
+      <c r="DZ77" s="8"/>
+      <c r="EA77" s="8"/>
+      <c r="EB77" s="8"/>
+      <c r="EC77" s="8"/>
+      <c r="ED77" s="8"/>
+      <c r="EE77" s="8"/>
+      <c r="EF77" s="8"/>
+      <c r="EG77" s="8"/>
+      <c r="EH77" s="8"/>
+      <c r="EI77" s="8"/>
+      <c r="EJ77" s="8"/>
+      <c r="EK77" s="8"/>
+      <c r="EL77" s="8"/>
+      <c r="EM77" s="8"/>
+      <c r="EN77" s="8"/>
+      <c r="EO77" s="8"/>
+      <c r="EP77" s="8"/>
+      <c r="EQ77" s="8"/>
+      <c r="ER77" s="8"/>
+      <c r="ES77" s="8"/>
+      <c r="ET77" s="8"/>
+      <c r="EU77" s="8"/>
+      <c r="EV77" s="8"/>
+      <c r="EW77" s="8"/>
+      <c r="EX77" s="8"/>
+      <c r="EY77" s="8"/>
+      <c r="EZ77" s="8"/>
+      <c r="FA77" s="8"/>
+      <c r="FB77" s="8"/>
+      <c r="FC77" s="8"/>
+      <c r="FD77" s="8"/>
+      <c r="FE77" s="8"/>
+      <c r="FF77" s="8"/>
+      <c r="FG77" s="8"/>
+      <c r="FH77" s="8"/>
+      <c r="FI77" s="8"/>
+      <c r="FJ77" s="8"/>
+      <c r="FK77" s="8"/>
+      <c r="FL77" s="8"/>
+      <c r="FM77" s="8"/>
+      <c r="FN77" s="8"/>
+      <c r="FO77" s="8"/>
+      <c r="FP77" s="8"/>
+      <c r="FQ77" s="8"/>
+      <c r="FR77" s="8"/>
+      <c r="FS77" s="8"/>
+      <c r="FT77" s="8"/>
+      <c r="FU77" s="8"/>
+      <c r="FV77" s="8"/>
+      <c r="FW77" s="8"/>
+      <c r="FX77" s="8"/>
+      <c r="FY77" s="8"/>
+      <c r="FZ77" s="8"/>
+      <c r="GA77" s="8"/>
+      <c r="GB77" s="8"/>
+      <c r="GC77" s="8"/>
+      <c r="GD77" s="8"/>
+      <c r="GE77" s="8"/>
+      <c r="GF77" s="8"/>
+      <c r="GG77" s="8"/>
+      <c r="GH77" s="8"/>
+      <c r="GI77" s="8"/>
+      <c r="GJ77" s="8"/>
+      <c r="GK77" s="8"/>
+      <c r="GL77" s="8"/>
+      <c r="GM77" s="8"/>
+      <c r="GN77" s="8"/>
+      <c r="GO77" s="8"/>
+      <c r="GP77" s="8"/>
+      <c r="GQ77" s="8"/>
+      <c r="GR77" s="8"/>
+      <c r="GS77" s="8"/>
+      <c r="GT77" s="8"/>
+      <c r="GU77" s="8"/>
+      <c r="GV77" s="8"/>
+      <c r="GW77" s="8"/>
+      <c r="GX77" s="8"/>
+      <c r="GY77" s="8"/>
+      <c r="GZ77" s="8"/>
+      <c r="HA77" s="8"/>
+      <c r="HB77" s="8"/>
+      <c r="HC77" s="8"/>
+      <c r="HD77" s="8"/>
+      <c r="HE77" s="8"/>
+      <c r="HF77" s="8"/>
+      <c r="HG77" s="8"/>
+      <c r="HH77" s="8"/>
+      <c r="HI77" s="8"/>
+      <c r="HJ77" s="8"/>
+      <c r="HK77" s="8"/>
+      <c r="HL77" s="8"/>
+      <c r="HM77" s="8"/>
+      <c r="HN77" s="8"/>
+      <c r="HO77" s="8"/>
+      <c r="HP77" s="8"/>
+      <c r="HQ77" s="8"/>
+      <c r="HR77" s="8"/>
+      <c r="HS77" s="8"/>
+      <c r="HT77" s="8"/>
+      <c r="HU77" s="8"/>
+      <c r="HV77" s="8"/>
+      <c r="HW77" s="8"/>
+      <c r="HX77" s="8"/>
+      <c r="HY77" s="8"/>
+      <c r="HZ77" s="8"/>
+      <c r="IA77" s="8"/>
+      <c r="IB77" s="8"/>
+      <c r="IC77" s="8"/>
+      <c r="ID77" s="8"/>
+      <c r="IE77" s="8"/>
+      <c r="IF77" s="8"/>
+      <c r="IG77" s="8"/>
+      <c r="IH77" s="8"/>
+      <c r="II77" s="8"/>
+      <c r="IJ77" s="8"/>
+      <c r="IK77" s="8"/>
+      <c r="IL77" s="8"/>
+      <c r="IM77" s="8"/>
+      <c r="IN77" s="8"/>
+      <c r="IO77" s="8"/>
+      <c r="IP77" s="8"/>
+      <c r="IQ77" s="8"/>
+      <c r="IR77" s="8"/>
+      <c r="IS77" s="8"/>
+      <c r="IT77" s="8"/>
+      <c r="IU77" s="8"/>
+      <c r="IV77" s="8"/>
+      <c r="IW77" s="8"/>
     </row>
     <row r="78" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
@@ -13965,7 +13888,7 @@
         <v>172902600</v>
       </c>
     </row>
-    <row r="79" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
         <v>1</v>
       </c>
@@ -14052,6 +13975,8 @@
       <c r="AC79" s="7" t="n">
         <v>42830</v>
       </c>
+      <c r="AD79" s="8"/>
+      <c r="AE79" s="8"/>
       <c r="AF79" s="0" t="n">
         <v>28176400</v>
       </c>
@@ -14594,91 +14519,91 @@
         <v>42838</v>
       </c>
     </row>
-    <row r="86" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="17" t="n">
+    <row r="86" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B86" s="18"/>
-      <c r="C86" s="17" t="s">
+      <c r="B86" s="16"/>
+      <c r="C86" s="2" t="s">
         <v>852</v>
       </c>
-      <c r="D86" s="19" t="n">
+      <c r="D86" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="E86" s="17" t="s">
+      <c r="E86" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="F86" s="20" t="n">
+      <c r="F86" s="5" t="n">
         <v>32470000</v>
       </c>
-      <c r="G86" s="17" t="s">
+      <c r="G86" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H86" s="20" t="n">
+      <c r="H86" s="5" t="n">
         <v>18342330</v>
       </c>
-      <c r="I86" s="17" t="s">
+      <c r="I86" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="J86" s="20" t="n">
+      <c r="J86" s="5" t="n">
         <v>12795250</v>
       </c>
-      <c r="K86" s="17" t="s">
+      <c r="K86" s="2" t="s">
         <v>853</v>
       </c>
-      <c r="L86" s="20" t="n">
+      <c r="L86" s="5" t="n">
         <v>9242200</v>
       </c>
-      <c r="M86" s="17" t="s">
+      <c r="M86" s="2" t="s">
         <v>854</v>
       </c>
-      <c r="N86" s="20" t="n">
+      <c r="N86" s="5" t="n">
         <v>9187500</v>
       </c>
-      <c r="O86" s="17" t="s">
+      <c r="O86" s="2" t="s">
         <v>855</v>
       </c>
-      <c r="P86" s="20" t="n">
+      <c r="P86" s="5" t="n">
         <v>6594100</v>
       </c>
-      <c r="Q86" s="17" t="s">
+      <c r="Q86" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="R86" s="20" t="n">
+      <c r="R86" s="5" t="n">
         <v>6212920</v>
       </c>
-      <c r="S86" s="21" t="s">
+      <c r="S86" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="T86" s="20" t="n">
+      <c r="T86" s="5" t="n">
         <v>6065400</v>
       </c>
-      <c r="U86" s="17" t="s">
+      <c r="U86" s="2" t="s">
         <v>858</v>
       </c>
-      <c r="V86" s="20" t="n">
+      <c r="V86" s="5" t="n">
         <v>4936200</v>
       </c>
-      <c r="W86" s="17" t="s">
+      <c r="W86" s="2" t="s">
         <v>859</v>
       </c>
-      <c r="X86" s="20" t="n">
+      <c r="X86" s="5" t="n">
         <v>4548300</v>
       </c>
-      <c r="Y86" s="20" t="n">
+      <c r="Y86" s="5" t="n">
         <f aca="false">SUM(E86:X86)</f>
         <v>110394200</v>
       </c>
-      <c r="Z86" s="22" t="n">
+      <c r="Z86" s="6" t="n">
         <v>2016</v>
       </c>
-      <c r="AA86" s="20" t="n">
+      <c r="AA86" s="5" t="n">
         <v>2168520572</v>
       </c>
-      <c r="AB86" s="20" t="n">
+      <c r="AB86" s="5" t="n">
         <v>2151066262</v>
       </c>
-      <c r="AC86" s="23" t="n">
+      <c r="AC86" s="7" t="n">
         <v>42888</v>
       </c>
     </row>
@@ -17731,7 +17656,7 @@
       <c r="AB122" s="5" t="n">
         <v>366624276</v>
       </c>
-      <c r="AC122" s="47" t="n">
+      <c r="AC122" s="32" t="n">
         <v>42849</v>
       </c>
     </row>
@@ -18272,16 +18197,16 @@
       <c r="D129" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="E129" s="48" t="s">
+      <c r="E129" s="33" t="s">
         <v>1242</v>
       </c>
-      <c r="F129" s="49" t="n">
+      <c r="F129" s="34" t="n">
         <v>42567580</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>1243</v>
       </c>
-      <c r="H129" s="49" t="n">
+      <c r="H129" s="34" t="n">
         <v>23450000</v>
       </c>
       <c r="I129" s="12" t="s">
@@ -18311,25 +18236,25 @@
       <c r="Q129" s="12" t="s">
         <v>1247</v>
       </c>
-      <c r="R129" s="49" t="n">
+      <c r="R129" s="34" t="n">
         <v>8864800</v>
       </c>
       <c r="S129" s="12" t="s">
         <v>1248</v>
       </c>
-      <c r="T129" s="49" t="n">
+      <c r="T129" s="34" t="n">
         <v>8482450</v>
       </c>
       <c r="U129" s="12" t="s">
         <v>1249</v>
       </c>
-      <c r="V129" s="49" t="n">
+      <c r="V129" s="34" t="n">
         <v>8464400</v>
       </c>
       <c r="W129" s="12" t="s">
         <v>1250</v>
       </c>
-      <c r="X129" s="49" t="n">
+      <c r="X129" s="34" t="n">
         <v>6478380</v>
       </c>
       <c r="Y129" s="11" t="n">
@@ -18695,7 +18620,7 @@
       <c r="AB133" s="11" t="n">
         <v>3828716963</v>
       </c>
-      <c r="AC133" s="50" t="n">
+      <c r="AC133" s="35" t="n">
         <v>41934</v>
       </c>
     </row>
@@ -19044,7 +18969,7 @@
       <c r="F138" s="5" t="n">
         <v>35466894</v>
       </c>
-      <c r="G138" s="51" t="s">
+      <c r="G138" s="36" t="s">
         <v>1326</v>
       </c>
       <c r="H138" s="5" t="n">
@@ -21333,7 +21258,7 @@
       <c r="E165" s="9" t="s">
         <v>1572</v>
       </c>
-      <c r="F165" s="37" t="n">
+      <c r="F165" s="29" t="n">
         <v>75569410</v>
       </c>
       <c r="G165" s="9" t="s">
@@ -21345,7 +21270,7 @@
       <c r="I165" s="9" t="s">
         <v>1574</v>
       </c>
-      <c r="J165" s="52" t="n">
+      <c r="J165" s="37" t="n">
         <v>58051391</v>
       </c>
       <c r="K165" s="9" t="s">
@@ -21497,7 +21422,7 @@
       <c r="C167" s="8" t="s">
         <v>1591</v>
       </c>
-      <c r="D167" s="53" t="n">
+      <c r="D167" s="38" t="n">
         <v>2015</v>
       </c>
       <c r="E167" s="8" t="s">
@@ -21506,13 +21431,13 @@
       <c r="F167" s="8" t="n">
         <v>10935550</v>
       </c>
-      <c r="G167" s="30" t="s">
+      <c r="G167" s="22" t="s">
         <v>1518</v>
       </c>
-      <c r="H167" s="30" t="n">
+      <c r="H167" s="22" t="n">
         <v>4516510</v>
       </c>
-      <c r="I167" s="54" t="s">
+      <c r="I167" s="31" t="s">
         <v>1592</v>
       </c>
       <c r="J167" s="8" t="n">
@@ -21560,11 +21485,11 @@
       <c r="X167" s="8" t="n">
         <v>2058120</v>
       </c>
-      <c r="Y167" s="54" t="n">
+      <c r="Y167" s="31" t="n">
         <f aca="false">SUM(F167:X167)</f>
         <v>36286064</v>
       </c>
-      <c r="Z167" s="54" t="n">
+      <c r="Z167" s="31" t="n">
         <v>2015</v>
       </c>
       <c r="AA167" s="8" t="n">
@@ -21573,7 +21498,7 @@
       <c r="AB167" s="8" t="n">
         <v>1279189398</v>
       </c>
-      <c r="AC167" s="55" t="n">
+      <c r="AC167" s="39" t="n">
         <v>42871</v>
       </c>
     </row>
@@ -21899,7 +21824,7 @@
       <c r="X172" s="11"/>
       <c r="Y172" s="11"/>
       <c r="Z172" s="13"/>
-      <c r="AA172" s="56"/>
+      <c r="AA172" s="40"/>
       <c r="AB172" s="11"/>
       <c r="AC172" s="14"/>
     </row>
@@ -23010,36 +22935,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="58.1836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="9" width="62.6377551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="9" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="11" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="11" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="13" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="11" width="20.25"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="11" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="14" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="257" min="30" style="9" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="57.5051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="9" width="61.8265306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="9" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="11" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="11" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="13" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="11" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="11" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="14" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="257" min="30" style="9" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26959,31 +26885,31 @@
       <c r="D46" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="E46" s="57" t="s">
+      <c r="E46" s="41" t="s">
         <v>468</v>
       </c>
       <c r="F46" s="5" t="n">
         <v>22238610</v>
       </c>
-      <c r="G46" s="27" t="s">
+      <c r="G46" s="19" t="s">
         <v>469</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>21993860</v>
       </c>
-      <c r="I46" s="27" t="s">
+      <c r="I46" s="19" t="s">
         <v>470</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>19242110</v>
       </c>
-      <c r="K46" s="27" t="s">
+      <c r="K46" s="19" t="s">
         <v>471</v>
       </c>
-      <c r="L46" s="28" t="n">
+      <c r="L46" s="20" t="n">
         <v>15487800</v>
       </c>
-      <c r="M46" s="27" t="s">
+      <c r="M46" s="19" t="s">
         <v>101</v>
       </c>
       <c r="N46" s="5" t="n">
@@ -26995,28 +26921,28 @@
       <c r="P46" s="5" t="n">
         <v>10859990</v>
       </c>
-      <c r="Q46" s="27" t="s">
+      <c r="Q46" s="19" t="s">
         <v>1781</v>
       </c>
       <c r="R46" s="5" t="n">
         <v>9840590</v>
       </c>
-      <c r="S46" s="57" t="s">
+      <c r="S46" s="41" t="s">
         <v>1782</v>
       </c>
       <c r="T46" s="5" t="n">
         <v>8776440</v>
       </c>
-      <c r="U46" s="27" t="s">
+      <c r="U46" s="19" t="s">
         <v>293</v>
       </c>
       <c r="V46" s="5" t="n">
         <v>8370880</v>
       </c>
-      <c r="W46" s="27" t="s">
+      <c r="W46" s="19" t="s">
         <v>1783</v>
       </c>
-      <c r="X46" s="28" t="n">
+      <c r="X46" s="20" t="n">
         <v>8184460</v>
       </c>
       <c r="Y46" s="5" t="n">
@@ -27636,7 +27562,7 @@
       <c r="AA53" s="5" t="n">
         <v>3594688850</v>
       </c>
-      <c r="AB53" s="31" t="n">
+      <c r="AB53" s="23" t="n">
         <v>3533281325</v>
       </c>
       <c r="AC53" s="7" t="n">
@@ -28153,7 +28079,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="24" t="s">
         <v>602</v>
       </c>
       <c r="D60" s="3" t="n">
@@ -28399,7 +28325,7 @@
       <c r="AA62" s="11" t="n">
         <v>904391025</v>
       </c>
-      <c r="AB62" s="33" t="n">
+      <c r="AB62" s="25" t="n">
         <v>901419307</v>
       </c>
       <c r="AC62" s="14" t="n">
@@ -28593,7 +28519,7 @@
       <c r="E65" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F65" s="34" t="n">
+      <c r="F65" s="26" t="n">
         <v>139442670</v>
       </c>
       <c r="G65" s="9" t="s">
@@ -28617,28 +28543,28 @@
       <c r="M65" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="N65" s="34" t="n">
+      <c r="N65" s="26" t="n">
         <v>48977640</v>
       </c>
-      <c r="O65" s="35" t="s">
+      <c r="O65" s="27" t="s">
         <v>658</v>
       </c>
       <c r="P65" s="11" t="n">
         <v>45400500</v>
       </c>
-      <c r="Q65" s="35" t="s">
+      <c r="Q65" s="27" t="s">
         <v>659</v>
       </c>
       <c r="R65" s="11" t="n">
         <v>44450000</v>
       </c>
-      <c r="S65" s="35" t="s">
+      <c r="S65" s="27" t="s">
         <v>660</v>
       </c>
       <c r="T65" s="11" t="n">
         <v>35652810</v>
       </c>
-      <c r="U65" s="35" t="s">
+      <c r="U65" s="27" t="s">
         <v>661</v>
       </c>
       <c r="V65" s="11" t="n">
@@ -28660,7 +28586,7 @@
       <c r="AA65" s="11" t="n">
         <v>3621429969</v>
       </c>
-      <c r="AB65" s="36" t="n">
+      <c r="AB65" s="28" t="n">
         <v>3535402755</v>
       </c>
       <c r="AC65" s="14" t="n">
@@ -29032,7 +28958,7 @@
       <c r="E70" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="F70" s="58" t="n">
+      <c r="F70" s="42" t="n">
         <v>109936552</v>
       </c>
       <c r="G70" s="2" t="s">
@@ -29091,7 +29017,7 @@
       <c r="Z70" s="6" t="n">
         <v>2014</v>
       </c>
-      <c r="AA70" s="59" t="n">
+      <c r="AA70" s="43" t="n">
         <v>1527677336</v>
       </c>
       <c r="AB70" s="5" t="n">
@@ -29501,7 +29427,7 @@
       <c r="AA75" s="11" t="n">
         <v>1034480809</v>
       </c>
-      <c r="AB75" s="52" t="n">
+      <c r="AB75" s="37" t="n">
         <v>1030897219</v>
       </c>
       <c r="AC75" s="14" t="n">
@@ -33396,7 +33322,7 @@
       <c r="AB122" s="5" t="n">
         <v>366726656</v>
       </c>
-      <c r="AC122" s="47" t="n">
+      <c r="AC122" s="32" t="n">
         <v>42166</v>
       </c>
     </row>
@@ -33930,16 +33856,16 @@
       <c r="D129" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="E129" s="48" t="s">
+      <c r="E129" s="33" t="s">
         <v>1242</v>
       </c>
-      <c r="F129" s="49" t="n">
+      <c r="F129" s="34" t="n">
         <v>42567580</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>1243</v>
       </c>
-      <c r="H129" s="49" t="n">
+      <c r="H129" s="34" t="n">
         <v>23450000</v>
       </c>
       <c r="I129" s="12" t="s">
@@ -33969,25 +33895,25 @@
       <c r="Q129" s="12" t="s">
         <v>1247</v>
       </c>
-      <c r="R129" s="49" t="n">
+      <c r="R129" s="34" t="n">
         <v>8864800</v>
       </c>
       <c r="S129" s="12" t="s">
         <v>1248</v>
       </c>
-      <c r="T129" s="49" t="n">
+      <c r="T129" s="34" t="n">
         <v>8482450</v>
       </c>
       <c r="U129" s="12" t="s">
         <v>1249</v>
       </c>
-      <c r="V129" s="49" t="n">
+      <c r="V129" s="34" t="n">
         <v>8464400</v>
       </c>
       <c r="W129" s="12" t="s">
         <v>1250</v>
       </c>
-      <c r="X129" s="49" t="n">
+      <c r="X129" s="34" t="n">
         <v>6478380</v>
       </c>
       <c r="Y129" s="11" t="n">
@@ -34355,7 +34281,7 @@
       <c r="AB133" s="5" t="n">
         <v>3828716963</v>
       </c>
-      <c r="AC133" s="60" t="n">
+      <c r="AC133" s="44" t="n">
         <v>41934</v>
       </c>
     </row>
@@ -34722,7 +34648,7 @@
       <c r="F138" s="5" t="n">
         <v>31034387</v>
       </c>
-      <c r="G138" s="51" t="s">
+      <c r="G138" s="36" t="s">
         <v>2067</v>
       </c>
       <c r="H138" s="5" t="n">
@@ -36986,7 +36912,7 @@
       <c r="E165" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="F165" s="58" t="n">
+      <c r="F165" s="42" t="n">
         <v>74746247</v>
       </c>
       <c r="G165" s="2" t="s">
@@ -36998,7 +36924,7 @@
       <c r="I165" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="J165" s="31" t="n">
+      <c r="J165" s="23" t="n">
         <v>60367098</v>
       </c>
       <c r="K165" s="2" t="s">
@@ -37148,7 +37074,7 @@
       <c r="C167" s="1" t="s">
         <v>1591</v>
       </c>
-      <c r="D167" s="61" t="n">
+      <c r="D167" s="45" t="n">
         <v>2014</v>
       </c>
       <c r="E167" s="1" t="s">
@@ -37157,7 +37083,7 @@
       <c r="F167" s="0" t="n">
         <v>10396340</v>
       </c>
-      <c r="G167" s="62" t="s">
+      <c r="G167" s="46" t="s">
         <v>1518</v>
       </c>
       <c r="H167" s="0" t="n">
@@ -37224,7 +37150,7 @@
       <c r="AB167" s="1" t="n">
         <v>1268176081</v>
       </c>
-      <c r="AC167" s="63" t="n">
+      <c r="AC167" s="47" t="n">
         <v>42140</v>
       </c>
       <c r="AD167" s="1"/>
@@ -37724,7 +37650,7 @@
       <c r="B171" s="16"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA172" s="56"/>
+      <c r="AA172" s="40"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="9" t="n">

</xml_diff>